<commit_message>
re-split excel sheets to individual files, updated readme, uploaded data to S3 and created DB in AWS
</commit_message>
<xml_diff>
--- a/data/Australia's Mothers and Babies 2018 - In Brief Supplementary Tables/Table 1.1.xlsx
+++ b/data/Australia's Mothers and Babies 2018 - In Brief Supplementary Tables/Table 1.1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d08107d86ebdc691/Desktop/Project/Maternal Health and Adoption/Australia's Mothers and Babies 2018 - In Brief Supplementary Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d08107d86ebdc691/Documents/GitHub/finalproject/data/Australia's Mothers and Babies 2018 - In Brief Supplementary Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4987E27-EA39-47D5-B3EE-E33DF4B74090}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A53E89F-8A74-449C-AAFD-0ABDC3209B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0DE6753B-E878-4B70-B84A-31FC36C397A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B6380503-ED3D-45F3-AF69-E788147F934F}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1.1" sheetId="1" r:id="rId1"/>
@@ -7349,7 +7349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934C8685-2BEE-4FF0-A9A8-BD62DB393747}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C521B6-E2F1-4452-818C-68F9942A1F0F}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>